<commit_message>
Updated NLP resume screening logic, unread filter, skill/experience match, Excel fix
</commit_message>
<xml_diff>
--- a/rejected_candidates.xlsx
+++ b/rejected_candidates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,16 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>matched_skills</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>required_skills</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>shortlisted</t>
         </is>
       </c>
@@ -478,37 +488,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rajesh.rajgor@example.com</t>
+          <t>rajeshrajgor025@gmail.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Application for Digital Marketing Executive Position</t>
+          <t>UI/UX APPLICATION JOB</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>google analytics, r, seo</t>
+          <t>machine learning, r</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>resumes\Marketing_Resume.pdf</t>
+          <t>resumes\Resume.pdf</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t># JD 3: Digital Marketing Executive
-Digital Marketing Executive: Looking for 0-3 years experience in...</t>
+          <t># JD 5: UI/UX Designer
+UI/UX Designer: Require 0–3 years of experience in user research, wireframing...</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>61.2</v>
-      </c>
-      <c r="H2" t="b">
+        <v>53.96</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>